<commit_message>
update excel add v2 for days
</commit_message>
<xml_diff>
--- a/insights/1/daily_submission_stats.xlsx
+++ b/insights/1/daily_submission_stats.xlsx
@@ -8,20 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\ioi_project\ioi-grant\insights\1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1A6D196-3BC6-4F7A-BBA4-7187262BB579}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06DD00CB-0740-42C0-BA9A-0E3B078BEA5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2019 DAY 1" sheetId="1" r:id="rId1"/>
-    <sheet name="2019 DAY 2" sheetId="2" r:id="rId2"/>
+    <sheet name="2019 DAY 1 V2" sheetId="3" r:id="rId1"/>
+    <sheet name="2019 DAY 2 V2" sheetId="4" r:id="rId2"/>
+    <sheet name="2019 DAY 1 V1" sheetId="1" r:id="rId3"/>
+    <sheet name="2019 DAY 2 V1" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="35">
   <si>
     <t>task</t>
   </si>
@@ -117,6 +119,15 @@
   </si>
   <si>
     <t>05:13:50</t>
+  </si>
+  <si>
+    <t>time_grp</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>count</t>
   </si>
 </sst>
 </file>
@@ -600,7 +611,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -612,6 +623,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -765,7 +779,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -803,7 +817,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$2:$K$2</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -867,7 +881,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -905,7 +919,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$3:$K$3</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -969,7 +983,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1007,7 +1021,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$4:$K$4</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1072,7 +1086,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1110,7 +1124,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$9:$K$9</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1175,7 +1189,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1213,7 +1227,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$10:$K$10</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1280,7 +1294,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 1'!$B$12:$K$12</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$12:$K$12</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -1318,7 +1332,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 1'!$B$11:$K$11</c:f>
+              <c:f>'2019 DAY 1 V1'!$B$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -1659,7 +1673,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1700,7 +1714,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$2:$L$2</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$2:$L$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1767,7 +1781,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1808,7 +1822,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$3:$L$3</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$3:$L$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1875,7 +1889,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -1916,7 +1930,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$4:$L$4</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$4:$L$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -1984,7 +1998,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2025,7 +2039,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$9:$L$9</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$9:$L$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2093,7 +2107,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2134,7 +2148,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$10:$L$10</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$10:$L$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -2204,7 +2218,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>'2019 DAY 2'!$B$5:$L$5</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$5:$L$5</c:f>
               <c:strCache>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
@@ -2245,7 +2259,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'2019 DAY 2'!$B$11:$L$11</c:f>
+              <c:f>'2019 DAY 2 V1'!$B$11:$L$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
@@ -3986,10 +4000,2551 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B2C5C76-BDD4-4FC5-AE26-802AE1A1A177}">
+  <dimension ref="A1:O33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="1">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="1">
+        <v>11</v>
+      </c>
+      <c r="I4" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="1">
+        <v>10</v>
+      </c>
+      <c r="M4" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="1">
+        <v>194</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1">
+        <v>163</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="1">
+        <v>55</v>
+      </c>
+      <c r="M5" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="1">
+        <v>13</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" s="1">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K6" s="1">
+        <v>4</v>
+      </c>
+      <c r="M6" s="5">
+        <v>43683.208333333336</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="1">
+        <v>38</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="1">
+        <v>12</v>
+      </c>
+      <c r="I7" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="1">
+        <v>9</v>
+      </c>
+      <c r="M7" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="1">
+        <v>288</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="1">
+        <v>234</v>
+      </c>
+      <c r="I8" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" s="1">
+        <v>107</v>
+      </c>
+      <c r="M8" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O8" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="1">
+        <v>50</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="1">
+        <v>18</v>
+      </c>
+      <c r="I9" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="1">
+        <v>5</v>
+      </c>
+      <c r="M9" s="5">
+        <v>43683.229166666664</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="1">
+        <v>94</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="1">
+        <v>47</v>
+      </c>
+      <c r="I10" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="1">
+        <v>19</v>
+      </c>
+      <c r="M10" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O10" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1">
+        <v>351</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="1">
+        <v>294</v>
+      </c>
+      <c r="I11" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K11" s="1">
+        <v>169</v>
+      </c>
+      <c r="M11" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O11" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="1">
+        <v>136</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="1">
+        <v>62</v>
+      </c>
+      <c r="I12" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="1">
+        <v>15</v>
+      </c>
+      <c r="M12" s="5">
+        <v>43683.25</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="1">
+        <v>132</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G13" s="1">
+        <v>72</v>
+      </c>
+      <c r="I13" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K13" s="1">
+        <v>52</v>
+      </c>
+      <c r="M13" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O13" s="1">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1">
+        <v>215</v>
+      </c>
+      <c r="E14" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G14" s="1">
+        <v>172</v>
+      </c>
+      <c r="I14" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K14" s="1">
+        <v>100</v>
+      </c>
+      <c r="M14" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O14" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="1">
+        <v>224</v>
+      </c>
+      <c r="E15" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1">
+        <v>95</v>
+      </c>
+      <c r="I15" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K15" s="1">
+        <v>23</v>
+      </c>
+      <c r="M15" s="5">
+        <v>43683.270833333336</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O15" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="1">
+        <v>158</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G16" s="1">
+        <v>87</v>
+      </c>
+      <c r="I16" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K16" s="1">
+        <v>58</v>
+      </c>
+      <c r="M16" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O16" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="1">
+        <v>263</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="1">
+        <v>216</v>
+      </c>
+      <c r="I17" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17" s="1">
+        <v>114</v>
+      </c>
+      <c r="M17" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O17" s="1">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1">
+        <v>308</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1">
+        <v>144</v>
+      </c>
+      <c r="I18" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1">
+        <v>64</v>
+      </c>
+      <c r="M18" s="5">
+        <v>43683.291666666664</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="1">
+        <v>194</v>
+      </c>
+      <c r="E19" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="1">
+        <v>101</v>
+      </c>
+      <c r="I19" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K19" s="1">
+        <v>62</v>
+      </c>
+      <c r="M19" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="1">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="1">
+        <v>157</v>
+      </c>
+      <c r="E20" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="1">
+        <v>137</v>
+      </c>
+      <c r="I20" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K20" s="1">
+        <v>63</v>
+      </c>
+      <c r="M20" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O20" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1">
+        <v>293</v>
+      </c>
+      <c r="E21" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="1">
+        <v>148</v>
+      </c>
+      <c r="I21" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1">
+        <v>65</v>
+      </c>
+      <c r="M21" s="5">
+        <v>43683.3125</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O21" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22" s="1">
+        <v>205</v>
+      </c>
+      <c r="E22" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G22" s="1">
+        <v>108</v>
+      </c>
+      <c r="I22" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K22" s="1">
+        <v>73</v>
+      </c>
+      <c r="M22" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O22" s="1">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="1">
+        <v>198</v>
+      </c>
+      <c r="E23" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G23" s="1">
+        <v>167</v>
+      </c>
+      <c r="I23" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K23" s="1">
+        <v>102</v>
+      </c>
+      <c r="M23" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O23" s="1">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" s="1">
+        <v>324</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="1">
+        <v>165</v>
+      </c>
+      <c r="I24" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24" s="1">
+        <v>66</v>
+      </c>
+      <c r="M24" s="5">
+        <v>43683.333333333336</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O24" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C25" s="1">
+        <v>259</v>
+      </c>
+      <c r="E25" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="1">
+        <v>143</v>
+      </c>
+      <c r="I25" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="1">
+        <v>84</v>
+      </c>
+      <c r="M25" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C26" s="1">
+        <v>142</v>
+      </c>
+      <c r="E26" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G26" s="1">
+        <v>121</v>
+      </c>
+      <c r="I26" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="1">
+        <v>62</v>
+      </c>
+      <c r="M26" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="1">
+        <v>367</v>
+      </c>
+      <c r="E27" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="1">
+        <v>211</v>
+      </c>
+      <c r="I27" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K27" s="1">
+        <v>99</v>
+      </c>
+      <c r="M27" s="5">
+        <v>43683.354166666664</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O27" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="1">
+        <v>348</v>
+      </c>
+      <c r="E28" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G28" s="1">
+        <v>179</v>
+      </c>
+      <c r="I28" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K28" s="1">
+        <v>116</v>
+      </c>
+      <c r="M28" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" s="1">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="1">
+        <v>151</v>
+      </c>
+      <c r="E29" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G29" s="1">
+        <v>115</v>
+      </c>
+      <c r="I29" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K29" s="1">
+        <v>57</v>
+      </c>
+      <c r="M29" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O29" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C30" s="1">
+        <v>316</v>
+      </c>
+      <c r="E30" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G30" s="1">
+        <v>164</v>
+      </c>
+      <c r="I30" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K30" s="1">
+        <v>62</v>
+      </c>
+      <c r="M30" s="5">
+        <v>43683.375</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1">
+        <v>521</v>
+      </c>
+      <c r="E31" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G31" s="1">
+        <v>308</v>
+      </c>
+      <c r="I31" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K31" s="1">
+        <v>190</v>
+      </c>
+      <c r="M31" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O31" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="1">
+        <v>198</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G32" s="1">
+        <v>155</v>
+      </c>
+      <c r="I32" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K32" s="1">
+        <v>77</v>
+      </c>
+      <c r="M32" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="O32" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="1">
+        <v>500</v>
+      </c>
+      <c r="E33" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G33" s="1">
+        <v>287</v>
+      </c>
+      <c r="I33" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K33" s="1">
+        <v>122</v>
+      </c>
+      <c r="M33" s="5">
+        <v>43683.395833333336</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O33" s="1">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55C23758-D2EE-4E8A-B50A-36E0B6162084}">
+  <dimension ref="A1:O36"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P10" sqref="P10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.42578125" customWidth="1"/>
+    <col min="13" max="13" width="14.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1">
+        <v>13</v>
+      </c>
+      <c r="E4" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="1">
+        <v>6</v>
+      </c>
+      <c r="I4" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="M4" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="1">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="1">
+        <v>6</v>
+      </c>
+      <c r="I5" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4</v>
+      </c>
+      <c r="M5" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0</v>
+      </c>
+      <c r="M6" s="5">
+        <v>43685.222222222219</v>
+      </c>
+      <c r="N6" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="1">
+        <v>85</v>
+      </c>
+      <c r="E7" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="1">
+        <v>58</v>
+      </c>
+      <c r="I7" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K7" s="1">
+        <v>14</v>
+      </c>
+      <c r="M7" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="1">
+        <v>134</v>
+      </c>
+      <c r="E8" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="1">
+        <v>79</v>
+      </c>
+      <c r="I8" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K8" s="1">
+        <v>45</v>
+      </c>
+      <c r="M8" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="1">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="I9" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+      <c r="M9" s="5">
+        <v>43685.243055555555</v>
+      </c>
+      <c r="N9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10" s="1">
+        <v>153</v>
+      </c>
+      <c r="E10" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1">
+        <v>115</v>
+      </c>
+      <c r="I10" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="1">
+        <v>50</v>
+      </c>
+      <c r="M10" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A11" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="1">
+        <v>282</v>
+      </c>
+      <c r="E11" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="1">
+        <v>169</v>
+      </c>
+      <c r="I11" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K11" s="1">
+        <v>111</v>
+      </c>
+      <c r="M11" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="N11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="1">
+        <v>41</v>
+      </c>
+      <c r="E12" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20</v>
+      </c>
+      <c r="I12" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="M12" s="5">
+        <v>43685.263888888891</v>
+      </c>
+      <c r="N12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O12" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1">
+        <v>212</v>
+      </c>
+      <c r="E13" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" s="1">
+        <v>178</v>
+      </c>
+      <c r="I13" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K13" s="1">
+        <v>103</v>
+      </c>
+      <c r="M13" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O13" s="1">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="1">
+        <v>275</v>
+      </c>
+      <c r="E14" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G14" s="1">
+        <v>138</v>
+      </c>
+      <c r="I14" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K14" s="1">
+        <v>80</v>
+      </c>
+      <c r="M14" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="N14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O14" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1">
+        <v>60</v>
+      </c>
+      <c r="E15" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="1">
+        <v>32</v>
+      </c>
+      <c r="I15" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K15" s="1">
+        <v>13</v>
+      </c>
+      <c r="M15" s="5">
+        <v>43685.284722222219</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O15" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="1">
+        <v>247</v>
+      </c>
+      <c r="E16" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" s="1">
+        <v>188</v>
+      </c>
+      <c r="I16" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1">
+        <v>119</v>
+      </c>
+      <c r="M16" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A17" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="1">
+        <v>339</v>
+      </c>
+      <c r="E17" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G17" s="1">
+        <v>153</v>
+      </c>
+      <c r="I17" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K17" s="1">
+        <v>91</v>
+      </c>
+      <c r="M17" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O17" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A18" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1">
+        <v>63</v>
+      </c>
+      <c r="E18" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G18" s="1">
+        <v>32</v>
+      </c>
+      <c r="I18" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K18" s="1">
+        <v>7</v>
+      </c>
+      <c r="M18" s="5">
+        <v>43685.305555555555</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O18" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="1">
+        <v>225</v>
+      </c>
+      <c r="E19" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G19" s="1">
+        <v>190</v>
+      </c>
+      <c r="I19" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1">
+        <v>124</v>
+      </c>
+      <c r="M19" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="1">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C20" s="1">
+        <v>262</v>
+      </c>
+      <c r="E20" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="1">
+        <v>132</v>
+      </c>
+      <c r="I20" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K20" s="1">
+        <v>78</v>
+      </c>
+      <c r="M20" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O20" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1">
+        <v>109</v>
+      </c>
+      <c r="E21" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="1">
+        <v>46</v>
+      </c>
+      <c r="I21" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K21" s="1">
+        <v>24</v>
+      </c>
+      <c r="M21" s="5">
+        <v>43685.326388888891</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O21" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1">
+        <v>260</v>
+      </c>
+      <c r="E22" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G22" s="1">
+        <v>205</v>
+      </c>
+      <c r="I22" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="1">
+        <v>136</v>
+      </c>
+      <c r="M22" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="1">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C23" s="1">
+        <v>212</v>
+      </c>
+      <c r="E23" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="1">
+        <v>116</v>
+      </c>
+      <c r="I23" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K23" s="1">
+        <v>67</v>
+      </c>
+      <c r="M23" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O23" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C24" s="1">
+        <v>165</v>
+      </c>
+      <c r="E24" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G24" s="1">
+        <v>71</v>
+      </c>
+      <c r="I24" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="J24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K24" s="1">
+        <v>26</v>
+      </c>
+      <c r="M24" s="5">
+        <v>43685.347222222219</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="1">
+        <v>279</v>
+      </c>
+      <c r="E25" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G25" s="1">
+        <v>236</v>
+      </c>
+      <c r="I25" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K25" s="1">
+        <v>186</v>
+      </c>
+      <c r="M25" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O25" s="1">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C26" s="1">
+        <v>214</v>
+      </c>
+      <c r="E26" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="1">
+        <v>109</v>
+      </c>
+      <c r="I26" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K26" s="1">
+        <v>62</v>
+      </c>
+      <c r="M26" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O26" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="1">
+        <v>167</v>
+      </c>
+      <c r="E27" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G27" s="1">
+        <v>72</v>
+      </c>
+      <c r="I27" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="1">
+        <v>26</v>
+      </c>
+      <c r="M27" s="5">
+        <v>43685.368055555555</v>
+      </c>
+      <c r="N27" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="1">
+        <v>351</v>
+      </c>
+      <c r="E28" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G28" s="1">
+        <v>314</v>
+      </c>
+      <c r="I28" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K28" s="1">
+        <v>233</v>
+      </c>
+      <c r="M28" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O28" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1">
+        <v>171</v>
+      </c>
+      <c r="E29" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="1">
+        <v>87</v>
+      </c>
+      <c r="I29" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K29" s="1">
+        <v>56</v>
+      </c>
+      <c r="M29" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="N29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O29" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A30" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C30" s="1">
+        <v>240</v>
+      </c>
+      <c r="E30" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G30" s="1">
+        <v>99</v>
+      </c>
+      <c r="I30" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K30" s="1">
+        <v>26</v>
+      </c>
+      <c r="M30" s="5">
+        <v>43685.388888888891</v>
+      </c>
+      <c r="N30" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O30" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A31" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C31" s="1">
+        <v>417</v>
+      </c>
+      <c r="E31" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G31" s="1">
+        <v>367</v>
+      </c>
+      <c r="I31" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K31" s="1">
+        <v>268</v>
+      </c>
+      <c r="M31" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O31" s="1">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C32" s="1">
+        <v>247</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G32" s="1">
+        <v>119</v>
+      </c>
+      <c r="I32" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K32" s="1">
+        <v>71</v>
+      </c>
+      <c r="M32" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="N32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O32" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C33" s="1">
+        <v>251</v>
+      </c>
+      <c r="E33" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G33" s="1">
+        <v>101</v>
+      </c>
+      <c r="I33" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K33" s="1">
+        <v>28</v>
+      </c>
+      <c r="M33" s="5">
+        <v>43685.409722222219</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O33" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A34" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C34" s="1">
+        <v>438</v>
+      </c>
+      <c r="E34" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G34" s="1">
+        <v>407</v>
+      </c>
+      <c r="I34" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K34" s="1">
+        <v>315</v>
+      </c>
+      <c r="M34" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="N34" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O34" s="1">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A35" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C35" s="1">
+        <v>228</v>
+      </c>
+      <c r="E35" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G35" s="1">
+        <v>119</v>
+      </c>
+      <c r="I35" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K35" s="1">
+        <v>81</v>
+      </c>
+      <c r="M35" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="O35" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C36" s="1">
+        <v>194</v>
+      </c>
+      <c r="E36" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G36" s="1">
+        <v>72</v>
+      </c>
+      <c r="I36" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K36" s="1">
+        <v>17</v>
+      </c>
+      <c r="M36" s="5">
+        <v>43685.430555555555</v>
+      </c>
+      <c r="N36" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O36" s="1">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
@@ -4705,7 +7260,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FFA2A15-FF93-4230-900A-E484501ECB63}">
   <dimension ref="A1:L26"/>
   <sheetViews>

</xml_diff>